<commit_message>
heatmap script w/ clustermap but w/o add'l flags
</commit_message>
<xml_diff>
--- a/pan_binary_heatmap.xlsx
+++ b/pan_binary_heatmap.xlsx
@@ -1237,15 +1237,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BS1" sqref="BS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="69" max="69" width="10.6640625" customWidth="1"/>
+    <col min="69" max="69" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.2">
@@ -22461,7 +22461,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>